<commit_message>
all data except memories and colors cleaned up
</commit_message>
<xml_diff>
--- a/MobileDB.xlsx
+++ b/MobileDB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Google Drive\Coding projects\pandas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Google Drive\Coding projects\mobinfo-database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9699CE88-7EA5-4EBB-AB66-323B9C7D7126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5634D31E-761E-4139-BDD7-85B3B23B64F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="552">
   <si>
     <t>Name</t>
   </si>
@@ -572,9 +572,6 @@
   </si>
   <si>
     <t>(Li-ion Non removable) 3000 mAh</t>
-  </si>
-  <si>
-    <t>Not Available</t>
   </si>
   <si>
     <t>4.7 stars - based on 1359 user reviews</t>
@@ -2490,8 +2487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I2" zoomScale="80" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="80" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2506,9 +2503,12 @@
     <col min="10" max="10" width="49" customWidth="1"/>
     <col min="11" max="11" width="32" customWidth="1"/>
     <col min="12" max="12" width="49.140625" customWidth="1"/>
-    <col min="13" max="13" width="4.42578125" customWidth="1"/>
-    <col min="14" max="16" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="145.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="15" max="15" width="103.140625" customWidth="1"/>
+    <col min="16" max="16" width="96.85546875" customWidth="1"/>
     <col min="17" max="17" width="83.5703125" customWidth="1"/>
+    <col min="18" max="18" width="45.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -3188,114 +3188,111 @@
       <c r="Q12" t="s">
         <v>183</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>184</v>
-      </c>
-      <c r="S12" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B13" t="s">
         <v>100</v>
       </c>
       <c r="C13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D13" t="s">
         <v>86</v>
       </c>
       <c r="E13" t="s">
+        <v>187</v>
+      </c>
+      <c r="F13" t="s">
         <v>188</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>189</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>190</v>
-      </c>
-      <c r="H13" t="s">
-        <v>191</v>
       </c>
       <c r="I13" t="s">
         <v>46</v>
       </c>
       <c r="J13" t="s">
+        <v>191</v>
+      </c>
+      <c r="L13" t="s">
         <v>192</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>193</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>194</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>195</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>196</v>
-      </c>
-      <c r="P13" t="s">
-        <v>197</v>
       </c>
       <c r="Q13" t="s">
         <v>54</v>
       </c>
       <c r="R13" t="s">
+        <v>197</v>
+      </c>
+      <c r="S13" t="s">
         <v>198</v>
-      </c>
-      <c r="S13" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B14" t="s">
         <v>100</v>
       </c>
       <c r="C14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D14" t="s">
         <v>59</v>
       </c>
       <c r="E14" t="s">
+        <v>201</v>
+      </c>
+      <c r="F14" t="s">
         <v>202</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>203</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>204</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>205</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>206</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>207</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>208</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>209</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>210</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>211</v>
-      </c>
-      <c r="O14" t="s">
-        <v>212</v>
       </c>
       <c r="P14" t="s">
         <v>81</v>
@@ -3304,27 +3301,27 @@
         <v>126</v>
       </c>
       <c r="R14" t="s">
+        <v>212</v>
+      </c>
+      <c r="S14" t="s">
         <v>213</v>
-      </c>
-      <c r="S14" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B15" t="s">
         <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D15" t="s">
         <v>144</v>
       </c>
       <c r="E15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F15" t="s">
         <v>60</v>
@@ -3333,137 +3330,137 @@
         <v>61</v>
       </c>
       <c r="H15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I15" t="s">
+        <v>216</v>
+      </c>
+      <c r="J15" t="s">
         <v>217</v>
-      </c>
-      <c r="J15" t="s">
-        <v>218</v>
       </c>
       <c r="L15" t="s">
         <v>49</v>
       </c>
       <c r="M15" t="s">
+        <v>218</v>
+      </c>
+      <c r="N15" t="s">
         <v>219</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>220</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>221</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>222</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>223</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>224</v>
-      </c>
-      <c r="S15" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D16" t="s">
+        <v>226</v>
+      </c>
+      <c r="E16" t="s">
         <v>227</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>228</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>229</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
+        <v>190</v>
+      </c>
+      <c r="I16" t="s">
         <v>230</v>
       </c>
-      <c r="H16" t="s">
-        <v>191</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>231</v>
       </c>
-      <c r="J16" t="s">
+      <c r="L16" t="s">
         <v>232</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>233</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>234</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>235</v>
-      </c>
-      <c r="O16" t="s">
-        <v>236</v>
       </c>
       <c r="P16" t="s">
         <v>96</v>
       </c>
       <c r="Q16" t="s">
+        <v>236</v>
+      </c>
+      <c r="R16" t="s">
         <v>237</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>238</v>
-      </c>
-      <c r="S16" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D17" t="s">
+        <v>240</v>
+      </c>
+      <c r="E17" t="s">
         <v>241</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>242</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>243</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>244</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>245</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>246</v>
       </c>
-      <c r="J17" t="s">
+      <c r="L17" t="s">
         <v>247</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>248</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
+        <v>234</v>
+      </c>
+      <c r="O17" t="s">
         <v>249</v>
-      </c>
-      <c r="N17" t="s">
-        <v>235</v>
-      </c>
-      <c r="O17" t="s">
-        <v>250</v>
       </c>
       <c r="P17" t="s">
         <v>68</v>
@@ -3472,51 +3469,51 @@
         <v>126</v>
       </c>
       <c r="R17" t="s">
+        <v>250</v>
+      </c>
+      <c r="S17" t="s">
         <v>251</v>
-      </c>
-      <c r="S17" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B18" t="s">
         <v>100</v>
       </c>
       <c r="D18" t="s">
+        <v>253</v>
+      </c>
+      <c r="E18" t="s">
         <v>254</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
+        <v>228</v>
+      </c>
+      <c r="G18" t="s">
+        <v>229</v>
+      </c>
+      <c r="H18" t="s">
+        <v>190</v>
+      </c>
+      <c r="I18" t="s">
+        <v>245</v>
+      </c>
+      <c r="J18" t="s">
         <v>255</v>
       </c>
-      <c r="F18" t="s">
-        <v>229</v>
-      </c>
-      <c r="G18" t="s">
-        <v>230</v>
-      </c>
-      <c r="H18" t="s">
-        <v>191</v>
-      </c>
-      <c r="I18" t="s">
-        <v>246</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="L18" t="s">
         <v>256</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>257</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
+        <v>234</v>
+      </c>
+      <c r="O18" t="s">
         <v>258</v>
-      </c>
-      <c r="N18" t="s">
-        <v>235</v>
-      </c>
-      <c r="O18" t="s">
-        <v>259</v>
       </c>
       <c r="P18" t="s">
         <v>152</v>
@@ -3525,817 +3522,817 @@
         <v>54</v>
       </c>
       <c r="R18" t="s">
+        <v>259</v>
+      </c>
+      <c r="S18" t="s">
         <v>260</v>
-      </c>
-      <c r="S18" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B19" t="s">
         <v>262</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>263</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>264</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>265</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
+        <v>242</v>
+      </c>
+      <c r="G19" t="s">
         <v>266</v>
       </c>
-      <c r="F19" t="s">
-        <v>243</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
+        <v>190</v>
+      </c>
+      <c r="I19" t="s">
         <v>267</v>
       </c>
-      <c r="H19" t="s">
-        <v>191</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>268</v>
-      </c>
-      <c r="J19" t="s">
-        <v>269</v>
       </c>
       <c r="L19" t="s">
         <v>105</v>
       </c>
       <c r="M19" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="P19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q19" t="s">
         <v>126</v>
       </c>
       <c r="R19" t="s">
+        <v>270</v>
+      </c>
+      <c r="S19" t="s">
         <v>271</v>
-      </c>
-      <c r="S19" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>272</v>
+      </c>
+      <c r="B20" t="s">
         <v>273</v>
       </c>
-      <c r="B20" t="s">
-        <v>274</v>
-      </c>
       <c r="C20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D20" t="s">
         <v>157</v>
       </c>
       <c r="E20" t="s">
+        <v>274</v>
+      </c>
+      <c r="F20" t="s">
         <v>275</v>
-      </c>
-      <c r="F20" t="s">
-        <v>276</v>
       </c>
       <c r="G20" t="s">
         <v>104</v>
       </c>
       <c r="H20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I20" t="s">
+        <v>276</v>
+      </c>
+      <c r="J20" t="s">
         <v>277</v>
       </c>
-      <c r="J20" t="s">
+      <c r="L20" t="s">
+        <v>256</v>
+      </c>
+      <c r="M20" t="s">
         <v>278</v>
       </c>
-      <c r="L20" t="s">
-        <v>257</v>
-      </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>279</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>280</v>
-      </c>
-      <c r="O20" t="s">
-        <v>281</v>
       </c>
       <c r="P20" t="s">
         <v>152</v>
       </c>
       <c r="Q20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="R20" t="s">
+        <v>281</v>
+      </c>
+      <c r="S20" t="s">
         <v>282</v>
-      </c>
-      <c r="S20" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>283</v>
+      </c>
+      <c r="B21" t="s">
+        <v>273</v>
+      </c>
+      <c r="C21" t="s">
         <v>284</v>
       </c>
-      <c r="B21" t="s">
-        <v>274</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>285</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>286</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>287</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>288</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>289</v>
-      </c>
-      <c r="H21" t="s">
-        <v>290</v>
       </c>
       <c r="I21" t="s">
         <v>62</v>
       </c>
       <c r="J21" t="s">
+        <v>290</v>
+      </c>
+      <c r="K21" t="s">
         <v>291</v>
-      </c>
-      <c r="K21" t="s">
-        <v>292</v>
       </c>
       <c r="L21" t="s">
         <v>64</v>
       </c>
       <c r="M21" t="s">
+        <v>292</v>
+      </c>
+      <c r="N21" t="s">
         <v>293</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>294</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>295</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>296</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" t="s">
         <v>297</v>
       </c>
-      <c r="R21" t="s">
+      <c r="S21" t="s">
         <v>298</v>
-      </c>
-      <c r="S21" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>299</v>
+      </c>
+      <c r="B22" t="s">
+        <v>273</v>
+      </c>
+      <c r="C22" t="s">
         <v>300</v>
       </c>
-      <c r="B22" t="s">
-        <v>274</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>301</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>302</v>
       </c>
-      <c r="E22" t="s">
-        <v>303</v>
-      </c>
       <c r="F22" t="s">
+        <v>287</v>
+      </c>
+      <c r="G22" t="s">
         <v>288</v>
       </c>
-      <c r="G22" t="s">
-        <v>289</v>
-      </c>
       <c r="H22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I22" t="s">
         <v>75</v>
       </c>
       <c r="J22" t="s">
+        <v>303</v>
+      </c>
+      <c r="K22" t="s">
         <v>304</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>305</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>306</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>307</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>308</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>309</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
+        <v>222</v>
+      </c>
+      <c r="R22" t="s">
         <v>310</v>
       </c>
-      <c r="Q22" t="s">
-        <v>223</v>
-      </c>
-      <c r="R22" t="s">
+      <c r="S22" t="s">
         <v>311</v>
-      </c>
-      <c r="S22" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>312</v>
+      </c>
+      <c r="B23" t="s">
         <v>313</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>314</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>315</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" t="s">
         <v>316</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>317</v>
-      </c>
-      <c r="H23" t="s">
-        <v>318</v>
       </c>
       <c r="I23" t="s">
         <v>75</v>
       </c>
       <c r="J23" t="s">
+        <v>318</v>
+      </c>
+      <c r="K23" t="s">
         <v>319</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>320</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>321</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>322</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>323</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
         <v>324</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>325</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="R23" t="s">
         <v>326</v>
       </c>
-      <c r="R23" t="s">
+      <c r="S23" t="s">
         <v>327</v>
-      </c>
-      <c r="S23" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>328</v>
+      </c>
+      <c r="B24" t="s">
         <v>329</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>330</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>331</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>332</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>333</v>
       </c>
-      <c r="G24" t="s">
-        <v>334</v>
-      </c>
       <c r="H24" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I24" t="s">
         <v>46</v>
       </c>
       <c r="J24" t="s">
+        <v>334</v>
+      </c>
+      <c r="K24" t="s">
         <v>335</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>336</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>337</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>338</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>339</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>340</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>341</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="R24" t="s">
         <v>342</v>
       </c>
-      <c r="R24" t="s">
+      <c r="S24" t="s">
         <v>343</v>
-      </c>
-      <c r="S24" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>344</v>
+      </c>
+      <c r="B25" t="s">
+        <v>313</v>
+      </c>
+      <c r="D25" t="s">
         <v>345</v>
       </c>
-      <c r="B25" t="s">
-        <v>314</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>315</v>
+      </c>
+      <c r="G25" t="s">
+        <v>316</v>
+      </c>
+      <c r="H25" t="s">
+        <v>317</v>
+      </c>
+      <c r="I25" t="s">
         <v>346</v>
       </c>
-      <c r="E25" t="s">
-        <v>316</v>
-      </c>
-      <c r="G25" t="s">
-        <v>317</v>
-      </c>
-      <c r="H25" t="s">
-        <v>318</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>347</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>348</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
+        <v>320</v>
+      </c>
+      <c r="M25" t="s">
         <v>349</v>
       </c>
-      <c r="L25" t="s">
-        <v>321</v>
-      </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>350</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>351</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q25" t="s">
         <v>352</v>
       </c>
-      <c r="P25" t="s">
-        <v>325</v>
-      </c>
-      <c r="Q25" t="s">
+      <c r="R25" t="s">
         <v>353</v>
       </c>
-      <c r="R25" t="s">
+      <c r="S25" t="s">
         <v>354</v>
-      </c>
-      <c r="S25" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>355</v>
+      </c>
+      <c r="B26" t="s">
+        <v>329</v>
+      </c>
+      <c r="D26" t="s">
+        <v>285</v>
+      </c>
+      <c r="E26" t="s">
+        <v>331</v>
+      </c>
+      <c r="F26" t="s">
+        <v>332</v>
+      </c>
+      <c r="G26" t="s">
+        <v>333</v>
+      </c>
+      <c r="H26" t="s">
+        <v>317</v>
+      </c>
+      <c r="I26" t="s">
         <v>356</v>
       </c>
-      <c r="B26" t="s">
-        <v>330</v>
-      </c>
-      <c r="D26" t="s">
-        <v>286</v>
-      </c>
-      <c r="E26" t="s">
-        <v>332</v>
-      </c>
-      <c r="F26" t="s">
-        <v>333</v>
-      </c>
-      <c r="G26" t="s">
-        <v>334</v>
-      </c>
-      <c r="H26" t="s">
-        <v>318</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>357</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
+        <v>335</v>
+      </c>
+      <c r="L26" t="s">
+        <v>336</v>
+      </c>
+      <c r="M26" t="s">
         <v>358</v>
       </c>
-      <c r="K26" t="s">
-        <v>336</v>
-      </c>
-      <c r="L26" t="s">
-        <v>337</v>
-      </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>359</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
+        <v>339</v>
+      </c>
+      <c r="P26" t="s">
         <v>360</v>
       </c>
-      <c r="O26" t="s">
-        <v>340</v>
-      </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>361</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="R26" t="s">
         <v>362</v>
       </c>
-      <c r="R26" t="s">
+      <c r="S26" t="s">
         <v>363</v>
-      </c>
-      <c r="S26" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>364</v>
+      </c>
+      <c r="B27" t="s">
         <v>365</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
         <v>366</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>367</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>368</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>369</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>370</v>
-      </c>
-      <c r="H27" t="s">
-        <v>371</v>
       </c>
       <c r="I27" t="s">
         <v>75</v>
       </c>
       <c r="J27" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K27" t="s">
+        <v>371</v>
+      </c>
+      <c r="L27" t="s">
+        <v>320</v>
+      </c>
+      <c r="M27" t="s">
         <v>372</v>
       </c>
-      <c r="L27" t="s">
-        <v>321</v>
-      </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>373</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>374</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
         <v>375</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
+        <v>551</v>
+      </c>
+      <c r="R27" t="s">
         <v>376</v>
       </c>
-      <c r="Q27" t="s">
-        <v>552</v>
-      </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
         <v>377</v>
-      </c>
-      <c r="S27" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>378</v>
+      </c>
+      <c r="B28" t="s">
+        <v>329</v>
+      </c>
+      <c r="D28" t="s">
         <v>379</v>
       </c>
-      <c r="B28" t="s">
-        <v>330</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>380</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
+        <v>332</v>
+      </c>
+      <c r="G28" t="s">
+        <v>333</v>
+      </c>
+      <c r="H28" t="s">
+        <v>317</v>
+      </c>
+      <c r="I28" t="s">
+        <v>356</v>
+      </c>
+      <c r="J28" t="s">
+        <v>357</v>
+      </c>
+      <c r="K28" t="s">
         <v>381</v>
       </c>
-      <c r="F28" t="s">
-        <v>333</v>
-      </c>
-      <c r="G28" t="s">
-        <v>334</v>
-      </c>
-      <c r="H28" t="s">
-        <v>318</v>
-      </c>
-      <c r="I28" t="s">
-        <v>357</v>
-      </c>
-      <c r="J28" t="s">
-        <v>358</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>382</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>383</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>384</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
+        <v>339</v>
+      </c>
+      <c r="P28" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>361</v>
+      </c>
+      <c r="R28" t="s">
         <v>385</v>
       </c>
-      <c r="O28" t="s">
-        <v>340</v>
-      </c>
-      <c r="P28" t="s">
-        <v>361</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>362</v>
-      </c>
-      <c r="R28" t="s">
+      <c r="S28" t="s">
         <v>386</v>
-      </c>
-      <c r="S28" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>387</v>
+      </c>
+      <c r="B29" t="s">
+        <v>313</v>
+      </c>
+      <c r="D29" t="s">
+        <v>285</v>
+      </c>
+      <c r="E29" t="s">
         <v>388</v>
       </c>
-      <c r="B29" t="s">
-        <v>314</v>
-      </c>
-      <c r="D29" t="s">
-        <v>286</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="G29" t="s">
+        <v>316</v>
+      </c>
+      <c r="H29" t="s">
         <v>389</v>
       </c>
-      <c r="G29" t="s">
-        <v>317</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
+        <v>356</v>
+      </c>
+      <c r="J29" t="s">
         <v>390</v>
       </c>
-      <c r="I29" t="s">
-        <v>357</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>391</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
+        <v>320</v>
+      </c>
+      <c r="M29" t="s">
         <v>392</v>
       </c>
-      <c r="L29" t="s">
-        <v>321</v>
-      </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>393</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>394</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q29" t="s">
         <v>395</v>
       </c>
-      <c r="P29" t="s">
-        <v>325</v>
-      </c>
-      <c r="Q29" t="s">
+      <c r="R29" t="s">
         <v>396</v>
       </c>
-      <c r="R29" t="s">
+      <c r="S29" t="s">
         <v>397</v>
-      </c>
-      <c r="S29" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>398</v>
+      </c>
+      <c r="B30" t="s">
+        <v>365</v>
+      </c>
+      <c r="D30" t="s">
         <v>399</v>
       </c>
-      <c r="B30" t="s">
-        <v>366</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>400</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
+        <v>368</v>
+      </c>
+      <c r="G30" t="s">
+        <v>369</v>
+      </c>
+      <c r="H30" t="s">
+        <v>190</v>
+      </c>
+      <c r="I30" t="s">
+        <v>356</v>
+      </c>
+      <c r="J30" t="s">
+        <v>390</v>
+      </c>
+      <c r="K30" t="s">
         <v>401</v>
       </c>
-      <c r="F30" t="s">
-        <v>369</v>
-      </c>
-      <c r="G30" t="s">
-        <v>370</v>
-      </c>
-      <c r="H30" t="s">
-        <v>191</v>
-      </c>
-      <c r="I30" t="s">
-        <v>357</v>
-      </c>
-      <c r="J30" t="s">
-        <v>391</v>
-      </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>402</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>403</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>404</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>405</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q30" t="s">
         <v>406</v>
       </c>
-      <c r="P30" t="s">
-        <v>341</v>
-      </c>
-      <c r="Q30" t="s">
+      <c r="R30" t="s">
         <v>407</v>
       </c>
-      <c r="R30" t="s">
+      <c r="S30" t="s">
         <v>408</v>
-      </c>
-      <c r="S30" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>409</v>
+      </c>
+      <c r="B31" t="s">
         <v>410</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
+        <v>345</v>
+      </c>
+      <c r="E31" t="s">
         <v>411</v>
       </c>
-      <c r="D31" t="s">
-        <v>346</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>412</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>413</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>414</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>415</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>416</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>417</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>418</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>419</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>420</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>421</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>422</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>423</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="R31" t="s">
         <v>424</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>425</v>
-      </c>
-      <c r="S31" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>426</v>
+      </c>
+      <c r="B32" t="s">
         <v>427</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
         <v>428</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>429</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>430</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>431</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
+        <v>370</v>
+      </c>
+      <c r="I32" t="s">
+        <v>346</v>
+      </c>
+      <c r="J32" t="s">
+        <v>347</v>
+      </c>
+      <c r="K32" t="s">
         <v>432</v>
       </c>
-      <c r="H32" t="s">
-        <v>371</v>
-      </c>
-      <c r="I32" t="s">
-        <v>347</v>
-      </c>
-      <c r="J32" t="s">
-        <v>348</v>
-      </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
+        <v>256</v>
+      </c>
+      <c r="M32" t="s">
         <v>433</v>
       </c>
-      <c r="L32" t="s">
-        <v>257</v>
-      </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>434</v>
       </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>435</v>
       </c>
-      <c r="O32" t="s">
+      <c r="P32" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q32" t="s">
         <v>436</v>
       </c>
-      <c r="P32" t="s">
-        <v>325</v>
-      </c>
-      <c r="Q32" t="s">
+      <c r="R32" t="s">
+        <v>424</v>
+      </c>
+      <c r="S32" t="s">
         <v>437</v>
-      </c>
-      <c r="R32" t="s">
-        <v>425</v>
-      </c>
-      <c r="S32" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B33" t="s">
         <v>39</v>
       </c>
       <c r="C33" t="s">
+        <v>439</v>
+      </c>
+      <c r="D33" t="s">
         <v>440</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>441</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>442</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>443</v>
       </c>
-      <c r="G33" t="s">
-        <v>444</v>
-      </c>
       <c r="H33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I33" t="s">
         <v>75</v>
@@ -4344,193 +4341,193 @@
         <v>76</v>
       </c>
       <c r="K33" t="s">
+        <v>444</v>
+      </c>
+      <c r="L33" t="s">
         <v>445</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>446</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>447</v>
       </c>
-      <c r="N33" t="s">
+      <c r="O33" t="s">
         <v>448</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
         <v>449</v>
-      </c>
-      <c r="P33" t="s">
-        <v>450</v>
       </c>
       <c r="Q33" t="s">
         <v>54</v>
       </c>
       <c r="R33" t="s">
+        <v>450</v>
+      </c>
+      <c r="S33" t="s">
         <v>451</v>
-      </c>
-      <c r="S33" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B34" t="s">
         <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D34" t="s">
+        <v>453</v>
+      </c>
+      <c r="E34" t="s">
         <v>454</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>455</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>456</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>457</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>458</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>459</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>460</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
+        <v>305</v>
+      </c>
+      <c r="M34" t="s">
         <v>461</v>
       </c>
-      <c r="L34" t="s">
-        <v>306</v>
-      </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>462</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>463</v>
-      </c>
-      <c r="O34" t="s">
-        <v>464</v>
       </c>
       <c r="P34" t="s">
         <v>81</v>
       </c>
       <c r="Q34" t="s">
+        <v>464</v>
+      </c>
+      <c r="R34" t="s">
+        <v>424</v>
+      </c>
+      <c r="S34" t="s">
         <v>465</v>
-      </c>
-      <c r="R34" t="s">
-        <v>425</v>
-      </c>
-      <c r="S34" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B35" t="s">
         <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D35" t="s">
+        <v>467</v>
+      </c>
+      <c r="E35" t="s">
         <v>468</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>469</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>470</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
+        <v>457</v>
+      </c>
+      <c r="I35" t="s">
         <v>471</v>
       </c>
-      <c r="H35" t="s">
-        <v>458</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>472</v>
-      </c>
-      <c r="J35" t="s">
-        <v>473</v>
       </c>
       <c r="L35" t="s">
         <v>64</v>
       </c>
       <c r="M35" t="s">
+        <v>473</v>
+      </c>
+      <c r="N35" t="s">
         <v>474</v>
       </c>
-      <c r="N35" t="s">
+      <c r="O35" t="s">
         <v>475</v>
       </c>
-      <c r="O35" t="s">
+      <c r="P35" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q35" t="s">
         <v>476</v>
       </c>
-      <c r="P35" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q35" t="s">
+      <c r="R35" t="s">
+        <v>223</v>
+      </c>
+      <c r="S35" t="s">
         <v>477</v>
-      </c>
-      <c r="R35" t="s">
-        <v>224</v>
-      </c>
-      <c r="S35" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B36" t="s">
         <v>39</v>
       </c>
       <c r="D36" t="s">
+        <v>479</v>
+      </c>
+      <c r="E36" t="s">
         <v>480</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>481</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>482</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>483</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>484</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>485</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>486</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>487</v>
       </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>488</v>
       </c>
-      <c r="M36" t="s">
+      <c r="N36" t="s">
         <v>489</v>
       </c>
-      <c r="N36" t="s">
+      <c r="O36" t="s">
         <v>490</v>
       </c>
-      <c r="O36" t="s">
-        <v>491</v>
-      </c>
       <c r="P36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q36" t="s">
         <v>54</v>
@@ -4539,319 +4536,319 @@
         <v>70</v>
       </c>
       <c r="S36" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B37" t="s">
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D37" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E37" t="s">
+        <v>493</v>
+      </c>
+      <c r="F37" t="s">
         <v>494</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>495</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
+        <v>483</v>
+      </c>
+      <c r="I37" t="s">
         <v>496</v>
       </c>
-      <c r="H37" t="s">
-        <v>484</v>
-      </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
+        <v>191</v>
+      </c>
+      <c r="K37" t="s">
         <v>497</v>
       </c>
-      <c r="J37" t="s">
-        <v>192</v>
-      </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
+        <v>305</v>
+      </c>
+      <c r="M37" t="s">
         <v>498</v>
       </c>
-      <c r="L37" t="s">
-        <v>306</v>
-      </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>499</v>
       </c>
-      <c r="N37" t="s">
+      <c r="O37" t="s">
         <v>500</v>
       </c>
-      <c r="O37" t="s">
+      <c r="P37" t="s">
         <v>501</v>
       </c>
-      <c r="P37" t="s">
+      <c r="Q37" t="s">
         <v>502</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="R37" t="s">
         <v>503</v>
       </c>
-      <c r="R37" t="s">
+      <c r="S37" t="s">
         <v>504</v>
-      </c>
-      <c r="S37" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B38" t="s">
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D38" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E38" t="s">
+        <v>506</v>
+      </c>
+      <c r="F38" t="s">
+        <v>469</v>
+      </c>
+      <c r="G38" t="s">
+        <v>470</v>
+      </c>
+      <c r="H38" t="s">
+        <v>483</v>
+      </c>
+      <c r="I38" t="s">
+        <v>496</v>
+      </c>
+      <c r="J38" t="s">
+        <v>191</v>
+      </c>
+      <c r="K38" t="s">
         <v>507</v>
-      </c>
-      <c r="F38" t="s">
-        <v>470</v>
-      </c>
-      <c r="G38" t="s">
-        <v>471</v>
-      </c>
-      <c r="H38" t="s">
-        <v>484</v>
-      </c>
-      <c r="I38" t="s">
-        <v>497</v>
-      </c>
-      <c r="J38" t="s">
-        <v>192</v>
-      </c>
-      <c r="K38" t="s">
-        <v>508</v>
       </c>
       <c r="L38" t="s">
         <v>49</v>
       </c>
       <c r="M38" t="s">
+        <v>508</v>
+      </c>
+      <c r="N38" t="s">
         <v>509</v>
       </c>
-      <c r="N38" t="s">
+      <c r="O38" t="s">
         <v>510</v>
       </c>
-      <c r="O38" t="s">
+      <c r="P38" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q38" t="s">
         <v>511</v>
       </c>
-      <c r="P38" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q38" t="s">
+      <c r="R38" t="s">
         <v>512</v>
       </c>
-      <c r="R38" t="s">
+      <c r="S38" t="s">
         <v>513</v>
-      </c>
-      <c r="S38" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B39" t="s">
         <v>20</v>
       </c>
       <c r="C39" t="s">
+        <v>515</v>
+      </c>
+      <c r="D39" t="s">
         <v>516</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>517</v>
-      </c>
-      <c r="E39" t="s">
-        <v>518</v>
       </c>
       <c r="F39" t="s">
         <v>60</v>
       </c>
       <c r="G39" t="s">
+        <v>518</v>
+      </c>
+      <c r="H39" t="s">
+        <v>190</v>
+      </c>
+      <c r="I39" t="s">
         <v>519</v>
       </c>
-      <c r="H39" t="s">
-        <v>191</v>
-      </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>520</v>
       </c>
-      <c r="J39" t="s">
+      <c r="K39" t="s">
         <v>521</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>522</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>523</v>
       </c>
-      <c r="M39" t="s">
+      <c r="N39" t="s">
         <v>524</v>
       </c>
-      <c r="N39" t="s">
+      <c r="O39" t="s">
         <v>525</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>511</v>
+      </c>
+      <c r="R39" t="s">
         <v>526</v>
       </c>
-      <c r="P39" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>512</v>
-      </c>
-      <c r="R39" t="s">
+      <c r="S39" t="s">
         <v>527</v>
-      </c>
-      <c r="S39" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B40" t="s">
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D40" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E40" t="s">
+        <v>529</v>
+      </c>
+      <c r="F40" t="s">
         <v>530</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>531</v>
-      </c>
-      <c r="G40" t="s">
-        <v>532</v>
       </c>
       <c r="H40" t="s">
         <v>45</v>
       </c>
       <c r="I40" t="s">
+        <v>532</v>
+      </c>
+      <c r="J40" t="s">
+        <v>485</v>
+      </c>
+      <c r="K40" t="s">
+        <v>486</v>
+      </c>
+      <c r="L40" t="s">
         <v>533</v>
       </c>
-      <c r="J40" t="s">
-        <v>486</v>
-      </c>
-      <c r="K40" t="s">
-        <v>487</v>
-      </c>
-      <c r="L40" t="s">
+      <c r="M40" t="s">
         <v>534</v>
       </c>
-      <c r="M40" t="s">
-        <v>535</v>
-      </c>
       <c r="N40" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="O40" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="P40" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q40" t="s">
         <v>54</v>
       </c>
       <c r="R40" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="S40" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B41" t="s">
         <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D41" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E41" t="s">
+        <v>537</v>
+      </c>
+      <c r="F41" t="s">
         <v>538</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>539</v>
       </c>
-      <c r="G41" t="s">
-        <v>540</v>
-      </c>
       <c r="H41" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I41" t="s">
         <v>75</v>
       </c>
       <c r="J41" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="K41" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L41" t="s">
         <v>64</v>
       </c>
       <c r="M41" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="N41" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="O41" t="s">
+        <v>541</v>
+      </c>
+      <c r="P41" t="s">
         <v>542</v>
       </c>
-      <c r="P41" t="s">
+      <c r="Q41" t="s">
         <v>543</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="R41" t="s">
+        <v>526</v>
+      </c>
+      <c r="S41" t="s">
         <v>544</v>
-      </c>
-      <c r="R41" t="s">
-        <v>527</v>
-      </c>
-      <c r="S41" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B42" t="s">
         <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D42" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E42" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F42" t="s">
         <v>60</v>
@@ -4860,40 +4857,40 @@
         <v>61</v>
       </c>
       <c r="H42" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I42" t="s">
+        <v>519</v>
+      </c>
+      <c r="J42" t="s">
         <v>520</v>
       </c>
-      <c r="J42" t="s">
-        <v>521</v>
-      </c>
       <c r="K42" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="L42" t="s">
         <v>105</v>
       </c>
       <c r="M42" t="s">
+        <v>547</v>
+      </c>
+      <c r="N42" t="s">
+        <v>524</v>
+      </c>
+      <c r="O42" t="s">
         <v>548</v>
       </c>
-      <c r="N42" t="s">
-        <v>525</v>
-      </c>
-      <c r="O42" t="s">
-        <v>549</v>
-      </c>
       <c r="P42" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="Q42" t="s">
         <v>54</v>
       </c>
       <c r="R42" t="s">
+        <v>549</v>
+      </c>
+      <c r="S42" t="s">
         <v>550</v>
-      </c>
-      <c r="S42" t="s">
-        <v>551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>